<commit_message>
v.6 I am sticking to stick and stones
</commit_message>
<xml_diff>
--- a/Metopen/Book1.xlsx
+++ b/Metopen/Book1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thinkin in programming\Metopen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF0800C-5446-47BB-A0E6-39731C88EF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98681CCC-F2F4-49BB-9D7C-30ADC719A093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11775" activeTab="2" xr2:uid="{252DCF02-E3DA-4351-BF14-229351A9F4F4}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11775" activeTab="3" xr2:uid="{252DCF02-E3DA-4351-BF14-229351A9F4F4}"/>
   </bookViews>
   <sheets>
     <sheet name="game window size" sheetId="1" r:id="rId1"/>
     <sheet name="sliding window Size" sheetId="2" r:id="rId2"/>
     <sheet name="ROI" sheetId="3" r:id="rId3"/>
+    <sheet name="desired ROI" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Game window Size</t>
   </si>
@@ -1062,6 +1063,445 @@
   </si>
   <si>
     <t>great</t>
+  </si>
+  <si>
+    <r>
+      <t>self</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>desired_roi_points</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>np</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>float32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>([</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>250</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Top-left</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>550</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Top-right</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>700</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-right</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">]   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-left</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>250</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Top-left (closer to 400px)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>750</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-right (closer to 780px)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-left</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
   </si>
 </sst>
 </file>
@@ -1375,6 +1815,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1402,6 +1848,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1415,33 +1882,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1768,10 +2208,10 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1779,58 +2219,58 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="22"/>
+      <c r="L2" s="24"/>
       <c r="M2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="21"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="K4" s="20" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="K4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="21"/>
+      <c r="L4" s="23"/>
       <c r="M4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="K6" s="20" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="K6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="21"/>
+      <c r="L6" s="23"/>
       <c r="M6" t="s">
         <v>12</v>
       </c>
@@ -1950,21 +2390,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C393B0EC-DECC-4367-BE98-AD590FB012B4}">
   <dimension ref="B3:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
@@ -1980,10 +2420,10 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="32"/>
+      <c r="I4" s="29"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
@@ -1993,8 +2433,8 @@
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -2005,8 +2445,8 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
       <c r="K6" t="s">
         <v>36</v>
       </c>
@@ -2020,8 +2460,8 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
@@ -2032,8 +2472,8 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
@@ -2044,8 +2484,8 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
@@ -2070,91 +2510,91 @@
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
       <c r="K14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="15" t="s">
         <v>29</v>
       </c>
       <c r="H22" t="s">
@@ -2165,17 +2605,17 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="15" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2193,4 +2633,87 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19C6A92-160B-4103-8D9F-1E10BB16CA6B}">
+  <dimension ref="B7:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v.7 Much Faster now
</commit_message>
<xml_diff>
--- a/Metopen/Book1.xlsx
+++ b/Metopen/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thinkin in programming\Metopen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98681CCC-F2F4-49BB-9D7C-30ADC719A093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB30463-E2BA-4A68-936C-279D0F868770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11775" activeTab="3" xr2:uid="{252DCF02-E3DA-4351-BF14-229351A9F4F4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Game window Size</t>
   </si>
@@ -1502,6 +1502,537 @@
   </si>
   <si>
     <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <r>
+      <t>monitor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"top"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: 300, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"left"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"width"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: 400, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"height"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: 300}</t>
+    </r>
+  </si>
+  <si>
+    <t>superb</t>
+  </si>
+  <si>
+    <r>
+      <t>            (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>137</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>127</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Top-left (274/2, 254/2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>258</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>127</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Top-right (517/2, 254/2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>374</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>156</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-right (748/2, 313/2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>156</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-left (13/2, 313/2)</t>
+    </r>
+  </si>
+  <si>
+    <t>400 * 300</t>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">],     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Top-left (100/2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>350</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Top-right (700/2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>350</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-right (700/2, 600/2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t># Bottom-left (100/2, 600/2)</t>
+    </r>
+  </si>
+  <si>
+    <t>meh</t>
   </si>
 </sst>
 </file>
@@ -2201,7 +2732,7 @@
   <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,8 +2811,23 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="L8" s="3"/>
+      <c r="B8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="K8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="23"/>
+      <c r="M8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -2333,7 +2879,9 @@
       <c r="L18" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="K8:L8"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B6:I6"/>
@@ -2388,10 +2936,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C393B0EC-DECC-4367-BE98-AD590FB012B4}">
-  <dimension ref="B3:K25"/>
+  <dimension ref="B3:K32"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,6 +3164,42 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" t="s">
+        <v>53</v>
+      </c>
+      <c r="K29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2637,10 +3221,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19C6A92-160B-4103-8D9F-1E10BB16CA6B}">
-  <dimension ref="B7:I22"/>
+  <dimension ref="B7:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2683,34 +3267,70 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>